<commit_message>
updating notes and training matrix score sheet
</commit_message>
<xml_diff>
--- a/ARC-Comm-ED-Training-Matrix-and-Scores.xlsx
+++ b/ARC-Comm-ED-Training-Matrix-and-Scores.xlsx
@@ -28,7 +28,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Kinder, Shannon:</t>
         </r>
@@ -37,7 +37,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 These should be combined into one training.  Introduction to SQL</t>
@@ -52,7 +52,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Kinder, Shannon:</t>
         </r>
@@ -61,7 +61,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 DTS is replaced by SSIS for 2005 and 2008, however, they still include the functionality but may not be supported in SQL Server 2012.</t>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="94">
   <si>
     <t>Topic</t>
   </si>
@@ -352,6 +352,24 @@
   </si>
   <si>
     <t>Best WID Practices (2.7)</t>
+  </si>
+  <si>
+    <t>Phil Ellsworth and?</t>
+  </si>
+  <si>
+    <t>David Lipnicky?</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>States using Tableau?</t>
+  </si>
+  <si>
+    <t>Look for notes from 2014 LMI Forum/ link to?</t>
+  </si>
+  <si>
+    <t>Allan and James? Chris?</t>
   </si>
 </sst>
 </file>
@@ -391,13 +409,13 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -509,6 +527,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -521,32 +545,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -849,14 +852,17 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="46.88671875" customWidth="1"/>
-    <col min="3" max="6" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" customWidth="1"/>
     <col min="7" max="7" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -864,12 +870,12 @@
       <c r="B1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1073,6 +1079,9 @@
       <c r="F11" s="18">
         <v>2.7</v>
       </c>
+      <c r="G11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1249,12 +1258,12 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="20" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="19" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1267,123 +1276,138 @@
       <c r="B30" t="s">
         <v>87</v>
       </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="19" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" s="23" t="s">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B46" s="23" t="s">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="19" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>76</v>
       </c>
@@ -1501,13 +1525,13 @@
       <c r="A8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1515,9 +1539,9 @@
       <c r="A9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
     </row>
     <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">

</xml_diff>